<commit_message>
added feature description + visual image of encoding
</commit_message>
<xml_diff>
--- a/CatanDB.xlsx
+++ b/CatanDB.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/niklasbille/projects/CatanAnalysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98D54454-7EDE-2C46-BE59-3BB052EB6D4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40304D2A-84E0-FA48-83B9-53CC6D7B7767}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{36430CA0-0917-3746-988E-C7102F59D220}"/>
+    <workbookView xWindow="14400" yWindow="500" windowWidth="14400" windowHeight="17500" activeTab="1" xr2:uid="{36430CA0-0917-3746-988E-C7102F59D220}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="127">
   <si>
     <t>Map string</t>
   </si>
@@ -65,21 +66,6 @@
     <t>PlayerFourPlacement</t>
   </si>
   <si>
-    <t>PlayerOnePoints</t>
-  </si>
-  <si>
-    <t>PlayerTwoPoints</t>
-  </si>
-  <si>
-    <t>PlayerThreePoints</t>
-  </si>
-  <si>
-    <t>PlayerFourPoints</t>
-  </si>
-  <si>
-    <t>WinningPlayer</t>
-  </si>
-  <si>
     <t>23-18, 40-45</t>
   </si>
   <si>
@@ -137,9 +123,6 @@
     <t>wh11,br12,or09,de00,sh06,sh05,wo10,br04,wo03,wh11,wo04,or08,wh08,sh10,sh9,br03,wh05,wo02,or06</t>
   </si>
   <si>
-    <t>Elo</t>
-  </si>
-  <si>
     <t>34-39,14-9</t>
   </si>
   <si>
@@ -159,18 +142,301 @@
   </si>
   <si>
     <t>wh9,or10,sh8,br12,sh5,de00,or3,sh11,wh06,wo11,or04,wo06,wh04,wo03,wo09,sh02,br08,sh10,br05</t>
+  </si>
+  <si>
+    <t>49-45,9-14</t>
+  </si>
+  <si>
+    <t>8-4,24-24-19</t>
+  </si>
+  <si>
+    <t>44-48,28-34</t>
+  </si>
+  <si>
+    <t>17-22, 47-43</t>
+  </si>
+  <si>
+    <t>wo,or,br,xx,xx,sh,xx,wh</t>
+  </si>
+  <si>
+    <t>wo5br10wh8or2sh9sh3sh4wh6sh4or11wh6wo11wo3wh5de0br12or8br10wo9</t>
+  </si>
+  <si>
+    <t>Player points</t>
+  </si>
+  <si>
+    <t>7,10,7,9</t>
+  </si>
+  <si>
+    <t>6,6,4,10</t>
+  </si>
+  <si>
+    <t>8,5,10,7</t>
+  </si>
+  <si>
+    <t>7,4,6,10</t>
+  </si>
+  <si>
+    <t>7,6,9,19</t>
+  </si>
+  <si>
+    <t>7,10,6,5</t>
+  </si>
+  <si>
+    <t>PointsFromSettlements</t>
+  </si>
+  <si>
+    <t>Points from cities</t>
+  </si>
+  <si>
+    <t>Points from VP cards</t>
+  </si>
+  <si>
+    <t>4,0,3,4</t>
+  </si>
+  <si>
+    <t>0,6,2,2</t>
+  </si>
+  <si>
+    <t>1,2,0,0</t>
+  </si>
+  <si>
+    <t>PlayerWithLargestArmy</t>
+  </si>
+  <si>
+    <t>PlayerWithLongestRoad</t>
+  </si>
+  <si>
+    <t>DiceStats</t>
+  </si>
+  <si>
+    <t>2,5,5,8,10,24,14,11,3,1,3</t>
+  </si>
+  <si>
+    <t>ResourceCardsDrawn</t>
+  </si>
+  <si>
+    <t>50,24,57,98,55</t>
+  </si>
+  <si>
+    <t>DiceStats ordering goes from 2-12</t>
+  </si>
+  <si>
+    <t>ResCardStats goes from wo, br, sh, wh, or</t>
+  </si>
+  <si>
+    <t>DevCardStats goes from knight, vp, mono, rb, yop</t>
+  </si>
+  <si>
+    <t>9-4,22-16</t>
+  </si>
+  <si>
+    <t>30-24,41-46</t>
+  </si>
+  <si>
+    <t>31-36,29-34</t>
+  </si>
+  <si>
+    <t>40-45, 20-25</t>
+  </si>
+  <si>
+    <t>5,10,6,5</t>
+  </si>
+  <si>
+    <t>5,2,2,3</t>
+  </si>
+  <si>
+    <t>0,6,4,2</t>
+  </si>
+  <si>
+    <t>0,0,0,0</t>
+  </si>
+  <si>
+    <t>3,3,2,6,7,9,6,7,3,2,2</t>
+  </si>
+  <si>
+    <t>45,32,38,35,36</t>
+  </si>
+  <si>
+    <t>sh,br,xx,xx,or,xx,wo,xx,wh</t>
+  </si>
+  <si>
+    <t>de0wh8wo5wo4wh3wh10sh2or11wo6sh11or9br6br12wh5or4br3sh9sh10wo8</t>
+  </si>
+  <si>
+    <t>ResourceStatsP1</t>
+  </si>
+  <si>
+    <t>ResourceStatsp2</t>
+  </si>
+  <si>
+    <t>ResourceStatsP4</t>
+  </si>
+  <si>
+    <t>ResourceStatsP3</t>
+  </si>
+  <si>
+    <t>42,15,27,34,3,0,5,4,1,0,10,0</t>
+  </si>
+  <si>
+    <t>66,25,41,56,3,0,7,10,7,0,8,0</t>
+  </si>
+  <si>
+    <t>50,23,27,37,2,0,11,0,1,0,22,0</t>
+  </si>
+  <si>
+    <t>49,19,30,38,3,0,8,5,2,0,12,0</t>
+  </si>
+  <si>
+    <t>31-25,39-34</t>
+  </si>
+  <si>
+    <t>41-45,35-30</t>
+  </si>
+  <si>
+    <t>14-19, 16-22</t>
+  </si>
+  <si>
+    <t>12-8, 24-18</t>
+  </si>
+  <si>
+    <t>5,4,4,10</t>
+  </si>
+  <si>
+    <t>3,1,2,5</t>
+  </si>
+  <si>
+    <t>2,2,2,2</t>
+  </si>
+  <si>
+    <t>0,1,0,1</t>
+  </si>
+  <si>
+    <t>1,5,6,8,6,6,15,5,2,1,1</t>
+  </si>
+  <si>
+    <t>50,28,55,35,32</t>
+  </si>
+  <si>
+    <t>ActivityStatsP2</t>
+  </si>
+  <si>
+    <t>ActivityStatsP1</t>
+  </si>
+  <si>
+    <t>ActivityStatsP4</t>
+  </si>
+  <si>
+    <t>ActivityStatsP3</t>
+  </si>
+  <si>
+    <t>11,2,23,1,2,2</t>
+  </si>
+  <si>
+    <t>0,0,28,1,7,4</t>
+  </si>
+  <si>
+    <t>9,2,15,1,0,0</t>
+  </si>
+  <si>
+    <t>12,2,42,1,1,0</t>
+  </si>
+  <si>
+    <t>51,27,24,39,2,0,10,0,1,5,21,0</t>
+  </si>
+  <si>
+    <t>54,21,33,34,3,11,6,0,3,0,18,0</t>
+  </si>
+  <si>
+    <t>37,21,16,29,1,0,7,4,1,4,12,0</t>
+  </si>
+  <si>
+    <t>81,40,41,66,3,0,12,4,4,2,30,0</t>
+  </si>
+  <si>
+    <t>xx,wh,xx,xx,xx,or,sh,wo,br</t>
+  </si>
+  <si>
+    <t>wh9wh12br11wo10sh5sh6wh4sh8de0sh11or3wo8br3br4or9or10wo6wh2wo5</t>
+  </si>
+  <si>
+    <t>ResourceStats ordering are:</t>
+  </si>
+  <si>
+    <t>Total ressource income</t>
+  </si>
+  <si>
+    <t>Total ressource loss</t>
+  </si>
+  <si>
+    <t>Total ressource score</t>
+  </si>
+  <si>
+    <t>Resouce gained by rolling dice</t>
+  </si>
+  <si>
+    <t>Ressource gained by robbing</t>
+  </si>
+  <si>
+    <t>Ressource gained by using dev cards</t>
+  </si>
+  <si>
+    <t>Ressource gained by trading</t>
+  </si>
+  <si>
+    <t>Ressource Lost by rolling 7</t>
+  </si>
+  <si>
+    <t>Ressource lost by getting robbed</t>
+  </si>
+  <si>
+    <t>Ressource lost by dev cards</t>
+  </si>
+  <si>
+    <t>Ressource lost by trading</t>
+  </si>
+  <si>
+    <t>Ressource gained by gold tiles</t>
+  </si>
+  <si>
+    <t>ActivityStats ordering:</t>
+  </si>
+  <si>
+    <t>Total times proposed to trade</t>
+  </si>
+  <si>
+    <t>Total successful trades with opponents</t>
+  </si>
+  <si>
+    <t>Amount of resources used</t>
+  </si>
+  <si>
+    <t>Amount of ressource income blocked</t>
+  </si>
+  <si>
+    <t>Amount of Dev cards bought</t>
+  </si>
+  <si>
+    <t>Amount of dev cards used</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -196,13 +462,13 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -224,23 +490,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>508000</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>88900</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>88900</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>139700</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
+        <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9894F847-0D71-B07D-E034-A6B65E555588}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2B6FD751-81B7-E947-967D-8A7DF4AB7B67}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -256,7 +522,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="23926800" y="469900"/>
+          <a:off x="3416300" y="6350000"/>
           <a:ext cx="7010400" cy="6578600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -586,10 +852,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87C339AD-142A-1A41-A84D-50BBD9E5CBA0}">
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:V9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -600,240 +866,516 @@
     <col min="4" max="4" width="19" customWidth="1"/>
     <col min="5" max="5" width="19.33203125" customWidth="1"/>
     <col min="6" max="6" width="18.5" customWidth="1"/>
-    <col min="7" max="7" width="14.5" customWidth="1"/>
-    <col min="8" max="8" width="15.5" customWidth="1"/>
-    <col min="9" max="9" width="17" customWidth="1"/>
-    <col min="10" max="10" width="16" customWidth="1"/>
-    <col min="11" max="11" width="13" customWidth="1"/>
-    <col min="12" max="12" width="7" customWidth="1"/>
+    <col min="7" max="7" width="19" customWidth="1"/>
+    <col min="8" max="8" width="22" customWidth="1"/>
+    <col min="9" max="9" width="21.5" customWidth="1"/>
+    <col min="10" max="10" width="22.1640625" customWidth="1"/>
+    <col min="11" max="11" width="20.6640625" customWidth="1"/>
+    <col min="12" max="12" width="20.1640625" customWidth="1"/>
+    <col min="13" max="13" width="23.33203125" customWidth="1"/>
+    <col min="14" max="14" width="13.5" customWidth="1"/>
+    <col min="15" max="16" width="12.5" customWidth="1"/>
+    <col min="17" max="17" width="12.6640625" customWidth="1"/>
+    <col min="18" max="18" width="13.5" customWidth="1"/>
+    <col min="19" max="19" width="25.5" customWidth="1"/>
+    <col min="20" max="20" width="24.6640625" customWidth="1"/>
+    <col min="21" max="21" width="25" customWidth="1"/>
+    <col min="22" max="22" width="27.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="S2" s="1"/>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H6" s="1"/>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C2" s="2" t="s">
+      <c r="D7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="K7">
+        <v>2</v>
+      </c>
+      <c r="L7">
         <v>1</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="M7" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="S7" s="1"/>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
         <v>2</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="2" t="s">
+      <c r="M8" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="S8" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="T8" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="U8" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="V8" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
         <v>4</v>
       </c>
-      <c r="G2" s="2">
-        <v>7</v>
-      </c>
-      <c r="H2" s="2">
-        <v>10</v>
-      </c>
-      <c r="I2">
-        <v>7</v>
-      </c>
-      <c r="J2">
-        <v>9</v>
-      </c>
-      <c r="K2">
-        <v>2</v>
-      </c>
-      <c r="L2">
-        <v>1335</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" s="2">
-        <v>6</v>
-      </c>
-      <c r="H3" s="2">
-        <v>6</v>
-      </c>
-      <c r="I3">
-        <v>4</v>
-      </c>
-      <c r="J3">
-        <v>10</v>
-      </c>
-      <c r="K3">
-        <v>4</v>
-      </c>
-      <c r="L3">
-        <v>1332</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G4" s="2">
-        <v>8</v>
-      </c>
-      <c r="H4" s="2">
-        <v>5</v>
-      </c>
-      <c r="I4">
-        <v>10</v>
-      </c>
-      <c r="J4">
-        <v>7</v>
-      </c>
-      <c r="K4">
-        <v>3</v>
-      </c>
-      <c r="L4">
-        <v>1330</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G5" s="2">
-        <v>7</v>
-      </c>
-      <c r="H5" s="2">
-        <v>4</v>
-      </c>
-      <c r="I5">
-        <v>6</v>
-      </c>
-      <c r="J5">
-        <v>10</v>
-      </c>
-      <c r="K5">
-        <v>4</v>
-      </c>
-      <c r="L5">
-        <v>1326</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="G6" s="2">
-        <v>7</v>
-      </c>
-      <c r="H6" s="2">
-        <v>6</v>
-      </c>
-      <c r="I6">
-        <v>9</v>
-      </c>
-      <c r="J6">
-        <v>19</v>
-      </c>
-      <c r="K6">
-        <v>4</v>
-      </c>
-      <c r="L6">
-        <v>1326</v>
+      <c r="M9" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q9" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="R9" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="S9" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="T9" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="U9" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="V9" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18083030-38C7-8F4C-9049-56F84FD42E43}">
+  <dimension ref="D3:D26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="11.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D6" s="3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="7" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="8" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D8" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="9" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D9" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="10" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D10" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="11" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D11" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="12" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D12" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="13" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D13" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="14" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D14" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="15" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D15" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="16" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D16" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="17" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D17" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="18" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D18" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="20" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D20" s="3" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="21" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D21" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="22" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D22" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="23" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D23" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="24" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D24" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="25" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D25" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="26" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D26" t="s">
+        <v>126</v>
       </c>
     </row>
   </sheetData>

</xml_diff>